<commit_message>
updated daily level sheet
</commit_message>
<xml_diff>
--- a/Healthify Excel Sheet.xlsx
+++ b/Healthify Excel Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\Healthify-NWMSU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F0CC70-B2F1-4E9C-AA08-25A8AC486C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6607B3C-2183-4182-A4DD-3EAA726C1217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,25 @@
     <sheet name="Group Member" sheetId="4" r:id="rId5"/>
     <sheet name="Challenge" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>Username</t>
   </si>
@@ -71,9 +79,6 @@
     <t>Step Count</t>
   </si>
   <si>
-    <t>Hydration</t>
-  </si>
-  <si>
     <t>Hours of Sleep</t>
   </si>
   <si>
@@ -201,6 +206,21 @@
   </si>
   <si>
     <t>672gbsgdj</t>
+  </si>
+  <si>
+    <t>Hydration(liters)</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Accepted</t>
   </si>
 </sst>
 </file>
@@ -208,8 +228,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -261,8 +281,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -548,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -614,13 +634,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" t="s">
         <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
       </c>
       <c r="D4" s="3">
         <v>43938</v>
@@ -631,13 +651,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
       </c>
       <c r="D5" s="5">
         <v>43956</v>
@@ -648,13 +668,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" t="s">
         <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>43974</v>
@@ -665,13 +685,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="D7" s="5">
         <v>43992</v>
@@ -682,13 +702,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" t="s">
         <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
       </c>
       <c r="D8" s="3">
         <v>44010</v>
@@ -699,13 +719,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" t="s">
         <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
       </c>
       <c r="D9" s="5">
         <v>44028</v>
@@ -716,13 +736,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" t="s">
         <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>53</v>
       </c>
       <c r="D10" s="3">
         <v>44046</v>
@@ -733,13 +753,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" t="s">
         <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
       </c>
       <c r="D11" s="3">
         <v>44064</v>
@@ -768,10 +788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20676B13-86C6-4AE2-9004-B6D76B7A80F9}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -793,19 +813,19 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -816,16 +836,236 @@
         <v>3452</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
         <v>8</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>350</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>218</v>
+      </c>
+      <c r="G2">
+        <f>+E2+F2</f>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>44043</v>
+      </c>
+      <c r="B3">
+        <v>7828</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>320</v>
+      </c>
+      <c r="F3">
+        <v>250</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G11" si="0">+E3+F3</f>
+        <v>570</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>44047</v>
+      </c>
+      <c r="B4">
+        <v>6000</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>420</v>
+      </c>
+      <c r="F4">
+        <v>290</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>710</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>44058</v>
+      </c>
+      <c r="B5">
+        <v>7500</v>
+      </c>
+      <c r="C5">
+        <v>2.5</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>360</v>
+      </c>
+      <c r="F5">
+        <v>220</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>44063</v>
+      </c>
+      <c r="B6">
+        <v>6500</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>290</v>
+      </c>
+      <c r="F6">
+        <v>350</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>44066</v>
+      </c>
+      <c r="B7">
+        <v>6472</v>
+      </c>
+      <c r="C7">
+        <v>2.8</v>
+      </c>
+      <c r="D7">
+        <v>6.5</v>
+      </c>
+      <c r="E7">
+        <v>209</v>
+      </c>
+      <c r="F7">
+        <v>420</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>44066</v>
+      </c>
+      <c r="B8">
+        <v>7200</v>
+      </c>
+      <c r="C8">
+        <v>2.6</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>467</v>
+      </c>
+      <c r="F8">
+        <v>299</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>766</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>44063</v>
+      </c>
+      <c r="B9">
+        <v>6738</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>527</v>
+      </c>
+      <c r="F9">
+        <v>201</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>728</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>44044</v>
+      </c>
+      <c r="B10">
+        <v>6389</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>7.5</v>
+      </c>
+      <c r="E10">
+        <v>268</v>
+      </c>
+      <c r="F10">
+        <v>479</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>747</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>44064</v>
+      </c>
+      <c r="B11">
+        <v>7863</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>638</v>
+      </c>
+      <c r="F11">
+        <v>493</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1131</v>
       </c>
     </row>
   </sheetData>
@@ -851,13 +1091,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -882,24 +1122,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5">
         <v>43975</v>
@@ -910,7 +1150,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -920,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D40A90-F5A4-4135-BFAE-25015617164A}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -936,20 +1176,161 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>44066</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>44066</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>44063</v>
+      </c>
+      <c r="B4" s="5">
+        <v>44064</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>44044</v>
+      </c>
+      <c r="B5" s="5">
+        <v>44044</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>44064</v>
+      </c>
+      <c r="B6" s="5">
+        <v>44065</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>44067</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>44043</v>
+      </c>
+      <c r="B8" s="5">
+        <v>44044</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="5">
+        <v>44063</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>44047</v>
+      </c>
+      <c r="B9" s="5">
+        <v>44048</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>44058</v>
+      </c>
+      <c r="B10" s="5">
+        <v>44063</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>44063</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="5">
+        <v>44064</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -971,16 +1352,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited in daily level sheet
</commit_message>
<xml_diff>
--- a/Healthify Excel Sheet.xlsx
+++ b/Healthify Excel Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\Healthify-NWMSU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6607B3C-2183-4182-A4DD-3EAA726C1217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAF0CA5-0C0F-4417-85C3-A5D8A6ACA36B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,12 +82,6 @@
     <t>Hours of Sleep</t>
   </si>
   <si>
-    <t>Fruit Servings</t>
-  </si>
-  <si>
-    <t>Vegetable Servings</t>
-  </si>
-  <si>
     <t>Total Calories</t>
   </si>
   <si>
@@ -221,6 +215,12 @@
   </si>
   <si>
     <t>Accepted</t>
+  </si>
+  <si>
+    <t>Fruit Servings(Cal)</t>
+  </si>
+  <si>
+    <t>Vegetable Servings(Cal)</t>
   </si>
 </sst>
 </file>
@@ -634,13 +634,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
       </c>
       <c r="D4" s="3">
         <v>43938</v>
@@ -651,13 +651,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
         <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
       </c>
       <c r="D5" s="5">
         <v>43956</v>
@@ -668,13 +668,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
       </c>
       <c r="D6" s="3">
         <v>43974</v>
@@ -685,13 +685,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="D7" s="5">
         <v>43992</v>
@@ -702,13 +702,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
       </c>
       <c r="D8" s="3">
         <v>44010</v>
@@ -719,13 +719,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
         <v>47</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
       </c>
       <c r="D9" s="5">
         <v>44028</v>
@@ -736,13 +736,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
       </c>
       <c r="D10" s="3">
         <v>44046</v>
@@ -753,13 +753,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
         <v>53</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
       </c>
       <c r="D11" s="3">
         <v>44064</v>
@@ -791,18 +791,18 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="1" max="1" width="16.90625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -813,19 +813,19 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1091,13 +1091,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1122,24 +1122,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5">
         <v>43975</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1176,16 +1176,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1193,13 +1193,13 @@
         <v>44066</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1207,13 +1207,13 @@
         <v>44066</v>
       </c>
       <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1224,10 +1224,10 @@
         <v>44064</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1238,10 +1238,10 @@
         <v>44044</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1252,10 +1252,10 @@
         <v>44065</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1263,13 +1263,13 @@
         <v>44067</v>
       </c>
       <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
         <v>57</v>
       </c>
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1280,7 +1280,7 @@
         <v>44044</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="5">
         <v>44063</v>
@@ -1294,10 +1294,10 @@
         <v>44048</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1308,10 +1308,10 @@
         <v>44063</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1319,13 +1319,13 @@
         <v>44063</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="5">
         <v>44064</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1352,16 +1352,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Group member sheet
</commit_message>
<xml_diff>
--- a/Healthify Excel Sheet.xlsx
+++ b/Healthify Excel Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\Healthify-NWMSU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAF0CA5-0C0F-4417-85C3-A5D8A6ACA36B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5C54DF-03EC-4465-9FAA-802D628EEE7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -285,6 +285,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -790,7 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20676B13-86C6-4AE2-9004-B6D76B7A80F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -1162,13 +1168,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D40A90-F5A4-4135-BFAE-25015617164A}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="17.81640625" customWidth="1"/>
     <col min="3" max="3" width="17.7265625" customWidth="1"/>
     <col min="4" max="4" width="14.26953125" customWidth="1"/>
@@ -1192,13 +1198,13 @@
       <c r="A2" s="5">
         <v>44066</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1206,13 +1212,13 @@
       <c r="A3" s="5">
         <v>44066</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1220,13 +1226,13 @@
       <c r="A4" s="5">
         <v>44063</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="8">
         <v>44064</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1234,13 +1240,13 @@
       <c r="A5" s="5">
         <v>44044</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="8">
         <v>44044</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1248,13 +1254,13 @@
       <c r="A6" s="5">
         <v>44064</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="8">
         <v>44065</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1262,13 +1268,13 @@
       <c r="A7" s="5">
         <v>44067</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1276,13 +1282,13 @@
       <c r="A8" s="5">
         <v>44043</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="8">
         <v>44044</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="8">
         <v>44063</v>
       </c>
     </row>
@@ -1290,13 +1296,13 @@
       <c r="A9" s="5">
         <v>44047</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="8">
         <v>44048</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1304,13 +1310,13 @@
       <c r="A10" s="5">
         <v>44058</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="8">
         <v>44063</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1318,13 +1324,13 @@
       <c r="A11" s="5">
         <v>44063</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="8">
         <v>44064</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated group member sheet
</commit_message>
<xml_diff>
--- a/Healthify Excel Sheet.xlsx
+++ b/Healthify Excel Sheet.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\Healthify-NWMSU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D1CFEE-8D88-4E5D-9DD1-36168B7B6958}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C97D5BB-BA3F-474A-A177-C45A745F341B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
     <sheet name="Daily level" sheetId="2" r:id="rId2"/>
     <sheet name="Group" sheetId="3" r:id="rId3"/>
     <sheet name="Group Member" sheetId="4" r:id="rId4"/>
-    <sheet name="Challenge" sheetId="5" r:id="rId5"/>
-    <sheet name="Target" sheetId="6" r:id="rId6"/>
+    <sheet name="Target" sheetId="6" r:id="rId5"/>
+    <sheet name="Challenge" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
   <si>
     <t>Username</t>
   </si>
@@ -690,7 +690,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -713,7 +713,7 @@
       <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -946,7 +946,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,8 +984,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>44067</v>
+      <c r="A2" s="9">
+        <v>43902</v>
       </c>
       <c r="B2" s="2">
         <v>3452</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
-        <v>44043</v>
+        <v>43920</v>
       </c>
       <c r="B3" s="2">
         <v>7828</v>
@@ -1032,8 +1032,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>44047</v>
+      <c r="A4" s="9">
+        <v>43938</v>
       </c>
       <c r="B4" s="2">
         <v>6000</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
-        <v>44058</v>
+        <v>43956</v>
       </c>
       <c r="B5" s="2">
         <v>7500</v>
@@ -1080,8 +1080,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>44063</v>
+      <c r="A6" s="9">
+        <v>43974</v>
       </c>
       <c r="B6" s="2">
         <v>6500</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
-        <v>44066</v>
+        <v>43992</v>
       </c>
       <c r="B7" s="2">
         <v>6472</v>
@@ -1128,8 +1128,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>44066</v>
+      <c r="A8" s="9">
+        <v>44010</v>
       </c>
       <c r="B8" s="2">
         <v>7200</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
-        <v>44063</v>
+        <v>44028</v>
       </c>
       <c r="B9" s="2">
         <v>6738</v>
@@ -1176,8 +1176,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>44044</v>
+      <c r="A10" s="9">
+        <v>44046</v>
       </c>
       <c r="B10" s="2">
         <v>6389</v>
@@ -1200,7 +1200,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+      <c r="A11" s="9">
         <v>44064</v>
       </c>
       <c r="B11" s="2">
@@ -1232,7 +1232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52822F6C-B1E2-4F42-9341-EA60F4278115}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1352,7 +1352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D40A90-F5A4-4135-BFAE-25015617164A}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1363,7 +1365,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1428,8 +1430,8 @@
       <c r="C5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>55</v>
+      <c r="D5" s="3">
+        <v>44058</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1523,10 +1525,139 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9DF7A7-E8E3-4FED-A01E-A1E8B4E43495}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.6328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.90625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="2">
+        <v>600000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711F9A07-984E-4336-B5F7-B020F799B24C}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1598,133 +1729,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9DF7A7-E8E3-4FED-A01E-A1E8B4E43495}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.6328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="2">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="2">
-        <v>600000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>